<commit_message>
shortrate and fxrate objects added
</commit_message>
<xml_diff>
--- a/Risk Driver Simulation/Runfiles/InflationInput.xlsx
+++ b/Risk Driver Simulation/Runfiles/InflationInput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JQ228YH\Documents\CVA Tool Python\CVA-Tool\Risk Driver Simulation\Runfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4A3801-1184-4E9B-B8FB-9AD2D8FA44E3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48AF075-495D-49A7-B85F-44440E2C17D9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Inflation1</t>
   </si>
@@ -126,25 +126,19 @@
     <t>Real Interest Rate</t>
   </si>
   <si>
-    <t>Nominal Interest Rate</t>
-  </si>
-  <si>
     <t>Starting Inflation Index</t>
   </si>
   <si>
     <t>Volatility real IR</t>
   </si>
   <si>
-    <t>Volatility nominal IR</t>
-  </si>
-  <si>
     <t>Volatility Index</t>
   </si>
   <si>
     <t>Mean reversion real</t>
   </si>
   <si>
-    <t>Mean reversion nominal</t>
+    <t>Nominal Interest Rate Reference</t>
   </si>
 </sst>
 </file>
@@ -462,15 +456,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD10"/>
+  <dimension ref="A1:AD8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" customWidth="1"/>
+    <col min="1" max="1" width="29.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
@@ -574,37 +568,27 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>